<commit_message>
add larger test dataset for admins
</commit_message>
<xml_diff>
--- a/inst/extdata/projects/simulated-data/simulated-data.xlsx
+++ b/inst/extdata/projects/simulated-data/simulated-data.xlsx
@@ -566,13 +566,13 @@
     <t xml:space="preserve">Johnston's Pond</t>
   </si>
   <si>
+    <t xml:space="preserve">Restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lobster Bay</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maintain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lobster Bay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore</t>
   </si>
   <si>
     <t xml:space="preserve">Port Joli</t>
@@ -1351,13 +1351,13 @@
         <v>10</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>429</v>
+        <v>487</v>
       </c>
     </row>
     <row r="5">
@@ -1374,13 +1374,13 @@
         <v>12</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>361</v>
+        <v>276</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>479</v>
+        <v>526</v>
       </c>
     </row>
     <row r="6">
@@ -1394,16 +1394,16 @@
         <v>43.8180985398522</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>333</v>
+        <v>268</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>313</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7">
@@ -1417,16 +1417,16 @@
         <v>43.5805904606311</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>208</v>
+        <v>290</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>432</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -1647,10 +1647,10 @@
         <v>25</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -1658,10 +1658,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -1669,10 +1669,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>43</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1752,13 +1752,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>192</v>
+        <v>141</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>198</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
@@ -1766,13 +1766,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>199</v>
+        <v>144</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6">
@@ -1780,13 +1780,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>170</v>
+        <v>197</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>137</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7">
@@ -1794,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>167</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1876,13 +1876,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>279</v>
+        <v>204</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>357</v>
+        <v>275</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>209</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5">
@@ -1890,13 +1890,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>282</v>
+        <v>377</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>305</v>
+        <v>392</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>273</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6">
@@ -1904,13 +1904,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>289</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7">
@@ -1918,13 +1918,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>315</v>
+        <v>388</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>383</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2000,13 +2000,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>392</v>
+        <v>573</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>332</v>
+        <v>485</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>437</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5">
@@ -2014,13 +2014,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>358</v>
+        <v>524</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>473</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6">
@@ -2028,13 +2028,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>504</v>
+        <v>358</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>371</v>
+        <v>540</v>
       </c>
     </row>
     <row r="7">
@@ -2042,13 +2042,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>546</v>
+        <v>337</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>492</v>
+        <v>468</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>409</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -2105,7 +2105,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -2145,7 +2145,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
update data with new whatdataio version
</commit_message>
<xml_diff>
--- a/inst/extdata/projects/simulated-data/simulated-data.xlsx
+++ b/inst/extdata/projects/simulated-data/simulated-data.xlsx
@@ -539,7 +539,7 @@
     <t xml:space="preserve">Please enter information for your sites into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input the longitude and latitude (in decimal degrees) of each site. If you have a shapefile with spatial locations (e.g. point localities, boundaries) of your sites, these can also be supplied in the NCC Priority Actions App. We also ask that you input the cost of implementing each management action (e.g. in Canadian Dollars) within each site. Please note that cost values should not be below zero (though they can equal zero) and not be greater than 1,000,000 (i.e. one million). As such, you might need to rescale your cost values. For example, if one of your cost values is “10000000” Canadian Dollars, instead of inputting values as Canadian Dollars, you could you input values as thousands of Canadian Dollars (i.e. “10000”). Please take care to ensure that all cost values are in the same units. After filling out this worksheet, every light gray cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input the longitude and latitude (in decimal degrees) of each site. If you have a shapefile with spatial locations (e.g. point localities, boundaries) of your sites, these can also be supplied in the What To Do application. We also ask that you input the cost of implementing each management action (e.g. in Canadian Dollars) within each site. Please note that cost values should not be below zero (though they can equal zero) and not be greater than 1,000,000 (i.e. one million). As such, you might need to rescale your cost values. For example, if one of your cost values is “10000000” Canadian Dollars, instead of inputting values as Canadian Dollars, you could you input values as thousands of Canadian Dollars (i.e. “10000”). Please take care to ensure that all cost values are in the same units. After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
     <t xml:space="preserve">Site ID</t>
@@ -572,6 +572,9 @@
     <t xml:space="preserve">Lobster Bay</t>
   </si>
   <si>
+    <t xml:space="preserve">Signage</t>
+  </si>
+  <si>
     <t xml:space="preserve">Port Joli</t>
   </si>
   <si>
@@ -581,7 +584,7 @@
     <t xml:space="preserve">Please enter feasibility information for your sites into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are feasible to implement within each site. By default, all actions can be potentially implemented within each and every site. To specify that a certain a certain action cannot be implemented within a certain site, please enter value of “0”. You can also ensure that a certain site can ONLY have a certain action implemented within it, by specifying a value of “0” for every other action. This information, if you prefer, can also be specified within the NCC Priority Actions App---however, you will have to re-specify this information each and every time you open the NCC Priority Actions App.</t>
+    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are feasible to implement within each site. By default, all actions can be potentially implemented within each and every site. To specify that a certain a certain action cannot be implemented within a certain site, please enter value of “0”. You can also ensure that a certain site can ONLY have a certain action implemented within it, by specifying a value of “0” for every other action. This information, if you prefer, can also be specified within the What To Do application---however, you will have to re-specify this information each and every time you open the application.</t>
   </si>
   <si>
     <t xml:space="preserve">Feasibility of “Maintain”</t>
@@ -672,9 +675,6 @@
   </si>
   <si>
     <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signage</t>
   </si>
   <si>
     <t xml:space="preserve">Bay in Nova Scotia</t>
@@ -1351,13 +1351,13 @@
         <v>10</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>355</v>
+        <v>371</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>328</v>
+        <v>596</v>
       </c>
     </row>
     <row r="5">
@@ -1371,21 +1371,21 @@
         <v>43.7654869380519</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>211</v>
+        <v>296</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>470</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>-64.9080895986714</v>
@@ -1397,18 +1397,18 @@
         <v>10</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>405</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>-65.3498991696735</v>
@@ -1417,16 +1417,16 @@
         <v>43.5805904606311</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>397</v>
+        <v>364</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>537</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -1490,7 +1490,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1498,7 +1498,7 @@
     <row r="2" ht="100" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1508,13 +1508,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
@@ -1547,7 +1547,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6" t="b">
         <v>1</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6" t="b">
         <v>1</v>
@@ -1620,59 +1620,59 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" ht="250" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>95</v>
+      </c>
+      <c r="C4" s="5" t="n">
         <v>24</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>76</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>81</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>91</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1720,7 +1720,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1728,7 +1728,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1738,13 +1738,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -1752,13 +1752,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>108</v>
+        <v>173</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>196</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
@@ -1766,41 +1766,41 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>196</v>
+        <v>141</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1844,7 +1844,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1852,7 +1852,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1862,13 +1862,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -1876,13 +1876,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>329</v>
+        <v>206</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>388</v>
+        <v>206</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>322</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5">
@@ -1890,41 +1890,41 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>271</v>
+        <v>379</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>346</v>
+        <v>207</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>304</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>335</v>
+        <v>396</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>325</v>
+        <v>298</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>337</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>363</v>
+        <v>287</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>274</v>
+        <v>229</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>375</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -1968,7 +1968,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1976,7 +1976,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1986,13 +1986,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -2000,13 +2000,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>551</v>
+        <v>373</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>551</v>
+        <v>441</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>357</v>
+        <v>463</v>
       </c>
     </row>
     <row r="5">
@@ -2014,41 +2014,41 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>318</v>
+        <v>397</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>494</v>
+        <v>369</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>596</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>384</v>
+        <v>542</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>457</v>
+        <v>506</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>561</v>
+        <v>514</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>564</v>
+        <v>600</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>506</v>
+        <v>481</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>406</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -2082,22 +2082,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
@@ -2105,19 +2105,19 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -2125,10 +2125,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
@@ -2142,13 +2142,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>50</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
update template format per https://github.com/NCC-CNC/whattemplatemaker/issues/23
</commit_message>
<xml_diff>
--- a/inst/extdata/projects/simulated-data/simulated-data.xlsx
+++ b/inst/extdata/projects/simulated-data/simulated-data.xlsx
@@ -9,9 +9,9 @@
     <sheet name="Site data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Feasibility data" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Feature data" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Consequence of “Maintain”" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Consequence of “Signage”" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Consequence of “Restore”" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="“Maintain” consequence" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="“Signage” consequence" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="“Restore” consequence" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="metadata" sheetId="7" state="hidden" r:id="rId7"/>
   </sheets>
 </workbook>
@@ -20,7 +20,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>X</author>
+    <author>What Template Maker</author>
   </authors>
   <commentList>
     <comment ref="E3" authorId="0" shapeId="0">
@@ -114,7 +114,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>X</author>
+    <author>What Template Maker</author>
   </authors>
   <commentList>
     <comment ref="B3" authorId="0" shapeId="0">
@@ -208,7 +208,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>X</author>
+    <author>What Template Maker</author>
   </authors>
   <commentList>
     <comment ref="A4" authorId="0" shapeId="0">
@@ -254,7 +254,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>X</author>
+    <author>What Template Maker</author>
   </authors>
   <commentList>
     <comment ref="B3" authorId="0" shapeId="0">
@@ -348,7 +348,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>X</author>
+    <author>What Template Maker</author>
   </authors>
   <commentList>
     <comment ref="B3" authorId="0" shapeId="0">
@@ -442,7 +442,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>X</author>
+    <author>What Template Maker</author>
   </authors>
   <commentList>
     <comment ref="B3" authorId="0" shapeId="0">
@@ -566,13 +566,13 @@
     <t xml:space="preserve">Johnston's Pond</t>
   </si>
   <si>
+    <t xml:space="preserve">Signage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lobster Bay</t>
+  </si>
+  <si>
     <t xml:space="preserve">Restore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lobster Bay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signage</t>
   </si>
   <si>
     <t xml:space="preserve">Port Joli</t>
@@ -1351,13 +1351,13 @@
         <v>10</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>174</v>
+        <v>141</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>371</v>
+        <v>238</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>596</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5">
@@ -1374,13 +1374,13 @@
         <v>12</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>527</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6">
@@ -1397,13 +1397,13 @@
         <v>10</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>207</v>
+        <v>329</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>363</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7">
@@ -1420,13 +1420,13 @@
         <v>12</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>520</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -1647,10 +1647,10 @@
         <v>25</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>24</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
@@ -1658,10 +1658,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -1669,10 +1669,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>27</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1752,13 +1752,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5">
@@ -1766,13 +1766,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
@@ -1780,13 +1780,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>157</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7">
@@ -1794,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>149</v>
+        <v>194</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>162</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1876,13 +1876,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>206</v>
+        <v>390</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>291</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5">
@@ -1890,13 +1890,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>379</v>
+        <v>282</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>237</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6">
@@ -1904,13 +1904,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>298</v>
+        <v>340</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>267</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7">
@@ -1918,13 +1918,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>287</v>
+        <v>221</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>229</v>
+        <v>323</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>251</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2000,13 +2000,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>441</v>
+        <v>376</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>463</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5">
@@ -2014,13 +2014,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
+        <v>520</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>519</v>
+      </c>
+      <c r="D5" s="5" t="n">
         <v>397</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>369</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>551</v>
       </c>
     </row>
     <row r="6">
@@ -2028,13 +2028,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>542</v>
+        <v>431</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>506</v>
+        <v>387</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>514</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7">
@@ -2042,13 +2042,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>600</v>
+        <v>410</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>481</v>
+        <v>405</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -2125,7 +2125,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -2145,7 +2145,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
update weights + site results table fix #47, fix #46, fix #42
</commit_message>
<xml_diff>
--- a/inst/extdata/projects/simulated-data/simulated-data.xlsx
+++ b/inst/extdata/projects/simulated-data/simulated-data.xlsx
@@ -566,18 +566,18 @@
     <t xml:space="preserve">Johnston's Pond</t>
   </si>
   <si>
+    <t xml:space="preserve">Restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lobster Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Joli</t>
+  </si>
+  <si>
     <t xml:space="preserve">Signage</t>
   </si>
   <si>
-    <t xml:space="preserve">Lobster Bay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port Joli</t>
-  </si>
-  <si>
     <t xml:space="preserve">Round Bay</t>
   </si>
   <si>
@@ -599,7 +599,7 @@
     <t xml:space="preserve">Please enter information for your features into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require percentage-based threshold values to specify the minimum amount of each feature you think is important to achieve across all of the sites (termed “goal”). Specifically, the goal values are expressed as a percentage of the maximum possible amount of each feature, assuming that the best possible action for each feature was implemented within each site (per the expecation data). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance (weight) of each feature. The default value is 1 such that all features are considered equally important. Greater values indicate greater importance. A weight of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Both goal and weight values should be between 0 and 100. Please note that these values can be changed later in the What To Do application. After filling out this worksheet, every light gray cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require percentage-based threshold values to specify the minimum amount of each feature you think is important to achieve across all of the sites (termed “goal”). Specifically, the goal values are expressed as a percentage of the maximum possible amount of each feature, assuming that the best possible action for each feature was implemented within each site (per the expecation data). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance of each feature. The default value is 1 such that all features are considered equally important. Greater values indicate greater importance. An importance value of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Both goal and importance values should be between 0 and 100. Please note that these values can be changed later in the What To Do application. After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
     <t xml:space="preserve">Feature ID</t>
@@ -608,7 +608,7 @@
     <t xml:space="preserve">Goal (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Relative importance (weight)</t>
+    <t xml:space="preserve">Relative importance</t>
   </si>
   <si>
     <t xml:space="preserve">Salt Marsh</t>
@@ -936,7 +936,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Feature ID"/>
     <tableColumn id="2" name="Goal (%)"/>
-    <tableColumn id="3" name="Relative importance (weight)"/>
+    <tableColumn id="3" name="Relative importance"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1351,13 +1351,13 @@
         <v>10</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>238</v>
+        <v>335</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5">
@@ -1371,21 +1371,21 @@
         <v>43.7654869380519</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>314</v>
+        <v>266</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>361</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>-64.9080895986714</v>
@@ -1394,16 +1394,16 @@
         <v>43.8180985398522</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>329</v>
+        <v>219</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>405</v>
+        <v>518</v>
       </c>
     </row>
     <row r="7">
@@ -1417,16 +1417,16 @@
         <v>43.5805904606311</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>338</v>
+        <v>215</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>354</v>
+        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="b">
         <v>1</v>
@@ -1614,7 +1614,7 @@
   <cols>
     <col min="1" max="1" width="28.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="18.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="38.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="29.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1647,10 +1647,10 @@
         <v>25</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>90</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
@@ -1658,10 +1658,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
@@ -1672,7 +1672,7 @@
         <v>99</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>92</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1752,13 +1752,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>122</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5">
@@ -1766,27 +1766,27 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>152</v>
+        <v>183</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>124</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>134</v>
+        <v>192</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>128</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7">
@@ -1794,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>194</v>
+        <v>116</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>118</v>
+        <v>181</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>140</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1876,13 +1876,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>390</v>
+        <v>230</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>223</v>
+        <v>280</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>335</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5">
@@ -1890,27 +1890,27 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>282</v>
+        <v>334</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>236</v>
+        <v>342</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>392</v>
+        <v>314</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>340</v>
+        <v>253</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>207</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7">
@@ -1918,13 +1918,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>221</v>
+        <v>340</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>323</v>
+        <v>285</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>301</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -2000,13 +2000,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>376</v>
+        <v>413</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>311</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5">
@@ -2014,27 +2014,27 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>520</v>
+        <v>454</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>519</v>
+        <v>558</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>397</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>431</v>
+        <v>483</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>387</v>
+        <v>507</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>363</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7">
@@ -2042,13 +2042,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>405</v>
+        <v>316</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>486</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -2125,7 +2125,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -2142,10 +2142,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>

</xml_diff>